<commit_message>
cracion de la clase cleaning
</commit_message>
<xml_diff>
--- a/muestra_datos.xlsx
+++ b/muestra_datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,37 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>character</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>vol</t>
+          <t>amiiboSeries</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>last</t>
+          <t>gameSeries</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>buy</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sell</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -479,26 +469,780 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>516099.66656665</v>
-      </c>
-      <c r="C2" t="n">
-        <v>479112.50000009</v>
-      </c>
-      <c r="D2" t="n">
-        <v>100.48629225</v>
-      </c>
-      <c r="E2" t="n">
-        <v>500062.36032481</v>
-      </c>
-      <c r="F2" t="n">
-        <v>499640.8898764</v>
-      </c>
-      <c r="G2" t="n">
-        <v>500239.26377885</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1740636736</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Metal Mario - Tennis</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Metal Mario</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Super Mario Cereal</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mario Cereal</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Kellogs</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Baby Mario - Soccer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Baby Mario</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Metal Mario - Soccer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Metal Mario</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mario - Soccer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Super Mario Bros.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>8-Bit Mario Modern Color</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>8-bit Mario</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Dr. Mario</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Super Smash Bros.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Baby Mario - Horse Racing</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Baby Mario</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mario - Cat</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Super Mario Bros.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Baby Mario - Golf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Baby Mario</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mario - Wedding</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Super Mario Bros.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Metal Mario - Golf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Metal Mario</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Super Smash Bros.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Mario - Tennis</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Baby Mario - Tennis</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Baby Mario</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mario - Gold Edition</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Super Mario Bros.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Mario - Power Up Band</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Super Nintendo World</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Band</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Metal Mario - Horse Racing</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Metal Mario</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Baby Mario - Baseball</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Baby Mario</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Mario - Golf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Mario - Silver Edition</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Super Mario Bros.</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Mario - Horse Racing</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>8-Bit Mario Classic Color</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>8-bit Mario</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Super Mario</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Figure</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Metal Mario - Baseball</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Metal Mario</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mario - Baseball</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Mario Sports Superstars</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>